<commit_message>
run the whole quarto report file
</commit_message>
<xml_diff>
--- a/data/Table of compounds_stringent_2025-04-18.xlsx
+++ b/data/Table of compounds_stringent_2025-04-18.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="687" documentId="11_C9C3E2DFE6E5ECF5CE906EFDC2549BB3DEDA2518" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{246463A5-2364-4429-A370-CB10D9D5C3C2}"/>
+  <xr:revisionPtr revIDLastSave="688" documentId="11_C9C3E2DFE6E5ECF5CE906EFDC2549BB3DEDA2518" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6C4FBAF6-6931-4CF4-A2F1-5FF3942F2A42}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="490" windowWidth="19200" windowHeight="10310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Experimental Design" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1533" uniqueCount="557">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1533" uniqueCount="558">
   <si>
     <t>Samples</t>
   </si>
@@ -1759,6 +1759,9 @@
   </si>
   <si>
     <t>Dose Response</t>
+  </si>
+  <si>
+    <t>Compound</t>
   </si>
 </sst>
 </file>
@@ -2735,7 +2738,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="373">
+  <cellXfs count="372">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -3223,26 +3226,38 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="10" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="10" borderId="46" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="10" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="10" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="10" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3253,94 +3268,37 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="50" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="51" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="11" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="11" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="11" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="9" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="9" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="50" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="51" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="10" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="10" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="10" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="46" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="50" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3367,12 +3325,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="11" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="11" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3421,58 +3373,108 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="46" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="10" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="10" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="10" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="11" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="50" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="51" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="9" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="9" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="50" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="51" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="10" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="10" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="10" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="46" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3634,7 +3636,7 @@
     <sortCondition ref="A1:A83"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{C833621C-1E47-4C45-8F7B-9F496D081E23}" name="Samples" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{C833621C-1E47-4C45-8F7B-9F496D081E23}" name="Compound" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{0569DB07-56D4-46A1-8998-DAE8B18F7DD3}" name="Samples_ID" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3936,7 +3938,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J271"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="C7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
@@ -3984,13 +3986,13 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="294" t="s">
+      <c r="A2" s="298" t="s">
         <v>141</v>
       </c>
-      <c r="B2" s="330" t="s">
+      <c r="B2" s="315" t="s">
         <v>140</v>
       </c>
-      <c r="C2" s="333"/>
+      <c r="C2" s="318"/>
       <c r="D2" s="4">
         <v>2</v>
       </c>
@@ -4010,9 +4012,9 @@
       <c r="J2" s="7"/>
     </row>
     <row r="3" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="295"/>
-      <c r="B3" s="331"/>
-      <c r="C3" s="334"/>
+      <c r="A3" s="299"/>
+      <c r="B3" s="316"/>
+      <c r="C3" s="319"/>
       <c r="D3" s="4">
         <v>2</v>
       </c>
@@ -4032,9 +4034,9 @@
       <c r="J3" s="8"/>
     </row>
     <row r="4" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="295"/>
-      <c r="B4" s="331"/>
-      <c r="C4" s="334"/>
+      <c r="A4" s="299"/>
+      <c r="B4" s="316"/>
+      <c r="C4" s="319"/>
       <c r="D4" s="5" t="s">
         <v>10</v>
       </c>
@@ -4054,9 +4056,9 @@
       <c r="J4" s="8"/>
     </row>
     <row r="5" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="295"/>
-      <c r="B5" s="331"/>
-      <c r="C5" s="334"/>
+      <c r="A5" s="299"/>
+      <c r="B5" s="316"/>
+      <c r="C5" s="319"/>
       <c r="D5" s="5" t="s">
         <v>10</v>
       </c>
@@ -4076,9 +4078,9 @@
       <c r="J5" s="8"/>
     </row>
     <row r="6" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="295"/>
-      <c r="B6" s="331"/>
-      <c r="C6" s="334"/>
+      <c r="A6" s="299"/>
+      <c r="B6" s="316"/>
+      <c r="C6" s="319"/>
       <c r="D6" s="5" t="s">
         <v>13</v>
       </c>
@@ -4098,9 +4100,9 @@
       <c r="J6" s="8"/>
     </row>
     <row r="7" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="295"/>
-      <c r="B7" s="331"/>
-      <c r="C7" s="334"/>
+      <c r="A7" s="299"/>
+      <c r="B7" s="316"/>
+      <c r="C7" s="319"/>
       <c r="D7" s="5" t="s">
         <v>13</v>
       </c>
@@ -4120,9 +4122,9 @@
       <c r="J7" s="8"/>
     </row>
     <row r="8" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="295"/>
-      <c r="B8" s="331"/>
-      <c r="C8" s="334"/>
+      <c r="A8" s="299"/>
+      <c r="B8" s="316"/>
+      <c r="C8" s="319"/>
       <c r="D8" s="285"/>
       <c r="E8" s="285"/>
       <c r="F8" t="s">
@@ -4142,9 +4144,9 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="295"/>
-      <c r="B9" s="331"/>
-      <c r="C9" s="335"/>
+      <c r="A9" s="299"/>
+      <c r="B9" s="316"/>
+      <c r="C9" s="320"/>
       <c r="D9" t="s">
         <v>13</v>
       </c>
@@ -4165,9 +4167,9 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="295"/>
-      <c r="B10" s="331"/>
-      <c r="C10" s="335"/>
+      <c r="A10" s="299"/>
+      <c r="B10" s="316"/>
+      <c r="C10" s="320"/>
       <c r="D10" s="202" t="s">
         <v>13</v>
       </c>
@@ -4187,9 +4189,9 @@
       <c r="J10" s="203"/>
     </row>
     <row r="11" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="295"/>
-      <c r="B11" s="332"/>
-      <c r="C11" s="336"/>
+      <c r="A11" s="299"/>
+      <c r="B11" s="317"/>
+      <c r="C11" s="321"/>
       <c r="D11" s="201" t="s">
         <v>13</v>
       </c>
@@ -4209,11 +4211,11 @@
       <c r="J11" s="204"/>
     </row>
     <row r="12" spans="1:10" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="295"/>
-      <c r="B12" s="352" t="s">
+      <c r="A12" s="299"/>
+      <c r="B12" s="335" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="333"/>
+      <c r="C12" s="318"/>
       <c r="D12" s="4" t="s">
         <v>18</v>
       </c>
@@ -4233,9 +4235,9 @@
       <c r="J12" s="7"/>
     </row>
     <row r="13" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="295"/>
-      <c r="B13" s="353"/>
-      <c r="C13" s="349"/>
+      <c r="A13" s="299"/>
+      <c r="B13" s="336"/>
+      <c r="C13" s="332"/>
       <c r="D13" s="5" t="s">
         <v>18</v>
       </c>
@@ -4255,9 +4257,9 @@
       <c r="J13" s="8"/>
     </row>
     <row r="14" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="295"/>
-      <c r="B14" s="353"/>
-      <c r="C14" s="349"/>
+      <c r="A14" s="299"/>
+      <c r="B14" s="336"/>
+      <c r="C14" s="332"/>
       <c r="D14" s="5" t="s">
         <v>18</v>
       </c>
@@ -4268,7 +4270,7 @@
       <c r="G14" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="H14" s="372" t="s">
+      <c r="H14" s="15" t="s">
         <v>546</v>
       </c>
       <c r="I14" s="9" t="s">
@@ -4277,9 +4279,9 @@
       <c r="J14" s="8"/>
     </row>
     <row r="15" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="295"/>
-      <c r="B15" s="353"/>
-      <c r="C15" s="349"/>
+      <c r="A15" s="299"/>
+      <c r="B15" s="336"/>
+      <c r="C15" s="332"/>
       <c r="D15" s="5" t="s">
         <v>18</v>
       </c>
@@ -4299,9 +4301,9 @@
       <c r="J15" s="8"/>
     </row>
     <row r="16" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="295"/>
-      <c r="B16" s="353"/>
-      <c r="C16" s="349"/>
+      <c r="A16" s="299"/>
+      <c r="B16" s="336"/>
+      <c r="C16" s="332"/>
       <c r="D16" s="5" t="s">
         <v>18</v>
       </c>
@@ -4321,9 +4323,9 @@
       <c r="J16" s="8"/>
     </row>
     <row r="17" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="295"/>
-      <c r="B17" s="353"/>
-      <c r="C17" s="349"/>
+      <c r="A17" s="299"/>
+      <c r="B17" s="336"/>
+      <c r="C17" s="332"/>
       <c r="D17" s="5" t="s">
         <v>18</v>
       </c>
@@ -4343,9 +4345,9 @@
       <c r="J17" s="8"/>
     </row>
     <row r="18" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="295"/>
-      <c r="B18" s="353"/>
-      <c r="C18" s="350"/>
+      <c r="A18" s="299"/>
+      <c r="B18" s="336"/>
+      <c r="C18" s="333"/>
       <c r="D18" s="12" t="s">
         <v>18</v>
       </c>
@@ -4365,9 +4367,9 @@
       <c r="J18" s="13"/>
     </row>
     <row r="19" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="295"/>
-      <c r="B19" s="353"/>
-      <c r="C19" s="350"/>
+      <c r="A19" s="299"/>
+      <c r="B19" s="336"/>
+      <c r="C19" s="333"/>
       <c r="D19" t="s">
         <v>18</v>
       </c>
@@ -4386,9 +4388,9 @@
       <c r="J19" s="284"/>
     </row>
     <row r="20" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="295"/>
-      <c r="B20" s="353"/>
-      <c r="C20" s="350"/>
+      <c r="A20" s="299"/>
+      <c r="B20" s="336"/>
+      <c r="C20" s="333"/>
       <c r="D20" s="24" t="s">
         <v>18</v>
       </c>
@@ -4408,9 +4410,9 @@
       <c r="J20" s="142"/>
     </row>
     <row r="21" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="295"/>
-      <c r="B21" s="353"/>
-      <c r="C21" s="350"/>
+      <c r="A21" s="299"/>
+      <c r="B21" s="336"/>
+      <c r="C21" s="333"/>
       <c r="D21" s="141" t="s">
         <v>18</v>
       </c>
@@ -4430,9 +4432,9 @@
       <c r="J21" s="143"/>
     </row>
     <row r="22" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="295"/>
-      <c r="B22" s="353"/>
-      <c r="C22" s="350"/>
+      <c r="A22" s="299"/>
+      <c r="B22" s="336"/>
+      <c r="C22" s="333"/>
       <c r="D22" s="120" t="s">
         <v>19</v>
       </c>
@@ -4454,9 +4456,9 @@
       </c>
     </row>
     <row r="23" spans="1:10" ht="15.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="295"/>
-      <c r="B23" s="353"/>
-      <c r="C23" s="351"/>
+      <c r="A23" s="299"/>
+      <c r="B23" s="336"/>
+      <c r="C23" s="334"/>
       <c r="D23" s="21" t="s">
         <v>18</v>
       </c>
@@ -4476,8 +4478,8 @@
       <c r="J23" s="142"/>
     </row>
     <row r="24" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="295"/>
-      <c r="B24" s="353"/>
+      <c r="A24" s="299"/>
+      <c r="B24" s="336"/>
       <c r="C24" s="273"/>
       <c r="D24" s="274" t="s">
         <v>18</v>
@@ -4500,8 +4502,8 @@
       </c>
     </row>
     <row r="25" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="295"/>
-      <c r="B25" s="353"/>
+      <c r="A25" s="299"/>
+      <c r="B25" s="336"/>
       <c r="C25" s="273"/>
       <c r="D25" s="274" t="s">
         <v>18</v>
@@ -4524,8 +4526,8 @@
       </c>
     </row>
     <row r="26" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="295"/>
-      <c r="B26" s="353"/>
+      <c r="A26" s="299"/>
+      <c r="B26" s="336"/>
       <c r="C26" s="273"/>
       <c r="D26" s="274" t="s">
         <v>10</v>
@@ -4548,8 +4550,8 @@
       </c>
     </row>
     <row r="27" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="296"/>
-      <c r="B27" s="354"/>
+      <c r="A27" s="300"/>
+      <c r="B27" s="337"/>
       <c r="C27" s="273"/>
       <c r="D27" s="274" t="s">
         <v>10</v>
@@ -4572,13 +4574,13 @@
       </c>
     </row>
     <row r="28" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="342" t="s">
+      <c r="A28" s="325" t="s">
         <v>25</v>
       </c>
-      <c r="B28" s="337" t="s">
+      <c r="B28" s="301" t="s">
         <v>143</v>
       </c>
-      <c r="C28" s="346" t="s">
+      <c r="C28" s="329" t="s">
         <v>24</v>
       </c>
       <c r="D28" s="122" t="s">
@@ -4604,9 +4606,9 @@
       </c>
     </row>
     <row r="29" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="343"/>
-      <c r="B29" s="358"/>
-      <c r="C29" s="347"/>
+      <c r="A29" s="326"/>
+      <c r="B29" s="302"/>
+      <c r="C29" s="330"/>
       <c r="D29" s="124" t="s">
         <v>18</v>
       </c>
@@ -4628,9 +4630,9 @@
       <c r="J29" s="126"/>
     </row>
     <row r="30" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="343"/>
-      <c r="B30" s="358"/>
-      <c r="C30" s="347"/>
+      <c r="A30" s="326"/>
+      <c r="B30" s="302"/>
+      <c r="C30" s="330"/>
       <c r="D30" s="127" t="s">
         <v>18</v>
       </c>
@@ -4652,9 +4654,9 @@
       <c r="J30" s="128"/>
     </row>
     <row r="31" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="343"/>
-      <c r="B31" s="358"/>
-      <c r="C31" s="347"/>
+      <c r="A31" s="326"/>
+      <c r="B31" s="302"/>
+      <c r="C31" s="330"/>
       <c r="D31" s="127" t="s">
         <v>18</v>
       </c>
@@ -4676,9 +4678,9 @@
       <c r="J31" s="128"/>
     </row>
     <row r="32" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="343"/>
-      <c r="B32" s="358"/>
-      <c r="C32" s="347"/>
+      <c r="A32" s="326"/>
+      <c r="B32" s="302"/>
+      <c r="C32" s="330"/>
       <c r="D32" s="127" t="s">
         <v>18</v>
       </c>
@@ -4702,9 +4704,9 @@
       </c>
     </row>
     <row r="33" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="343"/>
-      <c r="B33" s="358"/>
-      <c r="C33" s="347"/>
+      <c r="A33" s="326"/>
+      <c r="B33" s="302"/>
+      <c r="C33" s="330"/>
       <c r="D33" s="127" t="s">
         <v>18</v>
       </c>
@@ -4728,9 +4730,9 @@
       </c>
     </row>
     <row r="34" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="343"/>
-      <c r="B34" s="358"/>
-      <c r="C34" s="347"/>
+      <c r="A34" s="326"/>
+      <c r="B34" s="302"/>
+      <c r="C34" s="330"/>
       <c r="D34" s="127" t="s">
         <v>18</v>
       </c>
@@ -4754,9 +4756,9 @@
       </c>
     </row>
     <row r="35" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="343"/>
-      <c r="B35" s="358"/>
-      <c r="C35" s="347"/>
+      <c r="A35" s="326"/>
+      <c r="B35" s="302"/>
+      <c r="C35" s="330"/>
       <c r="D35" s="165" t="s">
         <v>18</v>
       </c>
@@ -4780,9 +4782,9 @@
       </c>
     </row>
     <row r="36" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="343"/>
-      <c r="B36" s="358"/>
-      <c r="C36" s="347"/>
+      <c r="A36" s="326"/>
+      <c r="B36" s="302"/>
+      <c r="C36" s="330"/>
       <c r="D36" s="165" t="s">
         <v>18</v>
       </c>
@@ -4806,9 +4808,9 @@
       </c>
     </row>
     <row r="37" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="343"/>
-      <c r="B37" s="358"/>
-      <c r="C37" s="347"/>
+      <c r="A37" s="326"/>
+      <c r="B37" s="302"/>
+      <c r="C37" s="330"/>
       <c r="D37" s="165" t="s">
         <v>18</v>
       </c>
@@ -4832,9 +4834,9 @@
       </c>
     </row>
     <row r="38" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="343"/>
-      <c r="B38" s="358"/>
-      <c r="C38" s="347"/>
+      <c r="A38" s="326"/>
+      <c r="B38" s="302"/>
+      <c r="C38" s="330"/>
       <c r="D38" s="165" t="s">
         <v>18</v>
       </c>
@@ -4858,9 +4860,9 @@
       </c>
     </row>
     <row r="39" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="343"/>
-      <c r="B39" s="358"/>
-      <c r="C39" s="347"/>
+      <c r="A39" s="326"/>
+      <c r="B39" s="302"/>
+      <c r="C39" s="330"/>
       <c r="D39" s="165" t="s">
         <v>18</v>
       </c>
@@ -4884,9 +4886,9 @@
       </c>
     </row>
     <row r="40" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="343"/>
-      <c r="B40" s="358"/>
-      <c r="C40" s="347"/>
+      <c r="A40" s="326"/>
+      <c r="B40" s="302"/>
+      <c r="C40" s="330"/>
       <c r="D40" s="165" t="s">
         <v>18</v>
       </c>
@@ -4910,9 +4912,9 @@
       </c>
     </row>
     <row r="41" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A41" s="343"/>
-      <c r="B41" s="358"/>
-      <c r="C41" s="348"/>
+      <c r="A41" s="326"/>
+      <c r="B41" s="302"/>
+      <c r="C41" s="331"/>
       <c r="D41" s="165" t="s">
         <v>73</v>
       </c>
@@ -4936,8 +4938,8 @@
       </c>
     </row>
     <row r="42" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="343"/>
-      <c r="B42" s="358"/>
+      <c r="A42" s="326"/>
+      <c r="B42" s="302"/>
       <c r="C42" s="137" t="s">
         <v>33</v>
       </c>
@@ -4964,8 +4966,8 @@
       </c>
     </row>
     <row r="43" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="343"/>
-      <c r="B43" s="358"/>
+      <c r="A43" s="326"/>
+      <c r="B43" s="302"/>
       <c r="C43" s="186" t="s">
         <v>211</v>
       </c>
@@ -4990,8 +4992,8 @@
       <c r="J43" s="192"/>
     </row>
     <row r="44" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="343"/>
-      <c r="B44" s="358"/>
+      <c r="A44" s="326"/>
+      <c r="B44" s="302"/>
       <c r="C44" s="186" t="s">
         <v>212</v>
       </c>
@@ -5016,8 +5018,8 @@
       <c r="J44" s="192"/>
     </row>
     <row r="45" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="343"/>
-      <c r="B45" s="358"/>
+      <c r="A45" s="326"/>
+      <c r="B45" s="302"/>
       <c r="C45" s="164" t="s">
         <v>213</v>
       </c>
@@ -5042,8 +5044,8 @@
       <c r="J45" s="193"/>
     </row>
     <row r="46" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="343"/>
-      <c r="B46" s="338"/>
+      <c r="A46" s="326"/>
+      <c r="B46" s="303"/>
       <c r="C46" s="280" t="s">
         <v>366</v>
       </c>
@@ -5068,11 +5070,11 @@
       <c r="J46" s="281"/>
     </row>
     <row r="47" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A47" s="343"/>
-      <c r="B47" s="337" t="s">
+      <c r="A47" s="326"/>
+      <c r="B47" s="301" t="s">
         <v>144</v>
       </c>
-      <c r="C47" s="345" t="s">
+      <c r="C47" s="328" t="s">
         <v>30</v>
       </c>
       <c r="D47" s="124" t="s">
@@ -5096,9 +5098,9 @@
       <c r="J47" s="126"/>
     </row>
     <row r="48" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="343"/>
-      <c r="B48" s="338"/>
-      <c r="C48" s="345"/>
+      <c r="A48" s="326"/>
+      <c r="B48" s="303"/>
+      <c r="C48" s="328"/>
       <c r="D48" s="131" t="s">
         <v>18</v>
       </c>
@@ -5120,7 +5122,7 @@
       <c r="J48" s="134"/>
     </row>
     <row r="49" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="343"/>
+      <c r="A49" s="326"/>
       <c r="B49" s="277"/>
       <c r="C49" s="278"/>
       <c r="D49" s="279" t="s">
@@ -5144,7 +5146,7 @@
       <c r="J49" s="281"/>
     </row>
     <row r="50" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="343"/>
+      <c r="A50" s="326"/>
       <c r="B50" s="277"/>
       <c r="C50" s="167" t="s">
         <v>142</v>
@@ -5170,7 +5172,7 @@
       <c r="J50" s="194"/>
     </row>
     <row r="51" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A51" s="344"/>
+      <c r="A51" s="327"/>
       <c r="B51" s="168" t="s">
         <v>145</v>
       </c>
@@ -5228,11 +5230,11 @@
       </c>
     </row>
     <row r="53" spans="1:10" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="339" t="s">
+      <c r="A53" s="322" t="s">
         <v>36</v>
       </c>
       <c r="B53" s="172"/>
-      <c r="C53" s="327" t="s">
+      <c r="C53" s="312" t="s">
         <v>35</v>
       </c>
       <c r="D53" s="63" t="s">
@@ -5256,9 +5258,9 @@
       <c r="J53" s="195"/>
     </row>
     <row r="54" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A54" s="340"/>
+      <c r="A54" s="323"/>
       <c r="B54" s="172"/>
-      <c r="C54" s="328"/>
+      <c r="C54" s="313"/>
       <c r="D54" s="66" t="s">
         <v>18</v>
       </c>
@@ -5280,9 +5282,9 @@
       <c r="J54" s="196"/>
     </row>
     <row r="55" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="340"/>
+      <c r="A55" s="323"/>
       <c r="B55" s="172"/>
-      <c r="C55" s="327" t="s">
+      <c r="C55" s="312" t="s">
         <v>37</v>
       </c>
       <c r="D55" s="63" t="s">
@@ -5306,9 +5308,9 @@
       <c r="J55" s="195"/>
     </row>
     <row r="56" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A56" s="340"/>
+      <c r="A56" s="323"/>
       <c r="B56" s="172"/>
-      <c r="C56" s="328"/>
+      <c r="C56" s="313"/>
       <c r="D56" s="66" t="s">
         <v>18</v>
       </c>
@@ -5330,7 +5332,7 @@
       <c r="J56" s="196"/>
     </row>
     <row r="57" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A57" s="340"/>
+      <c r="A57" s="323"/>
       <c r="B57" s="208"/>
       <c r="C57" s="209" t="s">
         <v>39</v>
@@ -5356,7 +5358,7 @@
       <c r="J57" s="213"/>
     </row>
     <row r="58" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A58" s="341"/>
+      <c r="A58" s="324"/>
       <c r="B58" s="109"/>
       <c r="C58" s="70" t="s">
         <v>215</v>
@@ -5382,11 +5384,11 @@
       <c r="J58" s="72"/>
     </row>
     <row r="59" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="305" t="s">
+      <c r="A59" s="291" t="s">
         <v>44</v>
       </c>
       <c r="B59" s="110"/>
-      <c r="C59" s="329" t="s">
+      <c r="C59" s="314" t="s">
         <v>42</v>
       </c>
       <c r="D59" s="4" t="s">
@@ -5410,9 +5412,9 @@
       <c r="J59" s="198"/>
     </row>
     <row r="60" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A60" s="305"/>
+      <c r="A60" s="291"/>
       <c r="B60" s="110"/>
-      <c r="C60" s="329"/>
+      <c r="C60" s="314"/>
       <c r="D60" s="5" t="s">
         <v>18</v>
       </c>
@@ -5434,9 +5436,9 @@
       <c r="J60" s="8"/>
     </row>
     <row r="61" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A61" s="305"/>
+      <c r="A61" s="291"/>
       <c r="B61" s="110"/>
-      <c r="C61" s="329"/>
+      <c r="C61" s="314"/>
       <c r="D61" s="12" t="s">
         <v>18</v>
       </c>
@@ -5458,7 +5460,7 @@
       <c r="J61" s="12"/>
     </row>
     <row r="62" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A62" s="306"/>
+      <c r="A62" s="290"/>
       <c r="B62" s="173"/>
       <c r="C62" s="36" t="s">
         <v>46</v>
@@ -5484,7 +5486,7 @@
       <c r="J62" s="42"/>
     </row>
     <row r="63" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="297" t="s">
+      <c r="A63" s="345" t="s">
         <v>51</v>
       </c>
       <c r="B63" s="111" t="s">
@@ -5516,7 +5518,7 @@
       </c>
     </row>
     <row r="64" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A64" s="298"/>
+      <c r="A64" s="346"/>
       <c r="B64" s="112" t="s">
         <v>51</v>
       </c>
@@ -5576,13 +5578,13 @@
       </c>
     </row>
     <row r="66" spans="1:10" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A66" s="307" t="s">
+      <c r="A66" s="352" t="s">
         <v>149</v>
       </c>
-      <c r="B66" s="312" t="s">
+      <c r="B66" s="357" t="s">
         <v>146</v>
       </c>
-      <c r="C66" s="317" t="s">
+      <c r="C66" s="362" t="s">
         <v>55</v>
       </c>
       <c r="D66" s="57" t="s">
@@ -5606,9 +5608,9 @@
       <c r="J66" s="57"/>
     </row>
     <row r="67" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="308"/>
-      <c r="B67" s="313"/>
-      <c r="C67" s="318"/>
+      <c r="A67" s="353"/>
+      <c r="B67" s="358"/>
+      <c r="C67" s="363"/>
       <c r="D67" s="46" t="s">
         <v>18</v>
       </c>
@@ -5630,9 +5632,9 @@
       <c r="J67" s="46"/>
     </row>
     <row r="68" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A68" s="308"/>
-      <c r="B68" s="313"/>
-      <c r="C68" s="318"/>
+      <c r="A68" s="353"/>
+      <c r="B68" s="358"/>
+      <c r="C68" s="363"/>
       <c r="D68" s="59" t="s">
         <v>18</v>
       </c>
@@ -5654,9 +5656,9 @@
       <c r="J68" s="59"/>
     </row>
     <row r="69" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A69" s="308"/>
-      <c r="B69" s="314"/>
-      <c r="C69" s="318"/>
+      <c r="A69" s="353"/>
+      <c r="B69" s="359"/>
+      <c r="C69" s="363"/>
       <c r="D69" s="15" t="s">
         <v>18</v>
       </c>
@@ -5680,9 +5682,9 @@
       </c>
     </row>
     <row r="70" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A70" s="308"/>
-      <c r="B70" s="314"/>
-      <c r="C70" s="318"/>
+      <c r="A70" s="353"/>
+      <c r="B70" s="359"/>
+      <c r="C70" s="363"/>
       <c r="D70" s="15" t="s">
         <v>18</v>
       </c>
@@ -5706,9 +5708,9 @@
       </c>
     </row>
     <row r="71" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A71" s="308"/>
-      <c r="B71" s="314"/>
-      <c r="C71" s="318"/>
+      <c r="A71" s="353"/>
+      <c r="B71" s="359"/>
+      <c r="C71" s="363"/>
       <c r="D71" s="15" t="s">
         <v>18</v>
       </c>
@@ -5732,9 +5734,9 @@
       </c>
     </row>
     <row r="72" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A72" s="308"/>
-      <c r="B72" s="314"/>
-      <c r="C72" s="318"/>
+      <c r="A72" s="353"/>
+      <c r="B72" s="359"/>
+      <c r="C72" s="363"/>
       <c r="D72" s="15" t="s">
         <v>18</v>
       </c>
@@ -5758,9 +5760,9 @@
       </c>
     </row>
     <row r="73" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A73" s="308"/>
-      <c r="B73" s="314"/>
-      <c r="C73" s="318"/>
+      <c r="A73" s="353"/>
+      <c r="B73" s="359"/>
+      <c r="C73" s="363"/>
       <c r="D73" s="15" t="s">
         <v>18</v>
       </c>
@@ -5784,9 +5786,9 @@
       </c>
     </row>
     <row r="74" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A74" s="308"/>
-      <c r="B74" s="314"/>
-      <c r="C74" s="319"/>
+      <c r="A74" s="353"/>
+      <c r="B74" s="359"/>
+      <c r="C74" s="364"/>
       <c r="D74" s="15" t="s">
         <v>18</v>
       </c>
@@ -5810,8 +5812,8 @@
       </c>
     </row>
     <row r="75" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A75" s="308"/>
-      <c r="B75" s="314"/>
+      <c r="A75" s="353"/>
+      <c r="B75" s="359"/>
       <c r="C75" s="236" t="s">
         <v>225</v>
       </c>
@@ -5836,8 +5838,8 @@
       <c r="J75" s="233"/>
     </row>
     <row r="76" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A76" s="308"/>
-      <c r="B76" s="315"/>
+      <c r="A76" s="353"/>
+      <c r="B76" s="360"/>
       <c r="C76" s="236" t="s">
         <v>226</v>
       </c>
@@ -5862,11 +5864,11 @@
       <c r="J76" s="233"/>
     </row>
     <row r="77" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A77" s="308"/>
-      <c r="B77" s="312" t="s">
+      <c r="A77" s="353"/>
+      <c r="B77" s="357" t="s">
         <v>147</v>
       </c>
-      <c r="C77" s="299" t="s">
+      <c r="C77" s="347" t="s">
         <v>59</v>
       </c>
       <c r="D77" s="57" t="s">
@@ -5890,9 +5892,9 @@
       <c r="J77" s="57"/>
     </row>
     <row r="78" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A78" s="308"/>
-      <c r="B78" s="313"/>
-      <c r="C78" s="300"/>
+      <c r="A78" s="353"/>
+      <c r="B78" s="358"/>
+      <c r="C78" s="348"/>
       <c r="D78" s="59" t="s">
         <v>18</v>
       </c>
@@ -5914,8 +5916,8 @@
       <c r="J78" s="59"/>
     </row>
     <row r="79" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A79" s="308"/>
-      <c r="B79" s="313"/>
+      <c r="A79" s="353"/>
+      <c r="B79" s="358"/>
       <c r="C79" s="170" t="s">
         <v>229</v>
       </c>
@@ -5940,8 +5942,8 @@
       <c r="J79" s="62"/>
     </row>
     <row r="80" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A80" s="308"/>
-      <c r="B80" s="316"/>
+      <c r="A80" s="353"/>
+      <c r="B80" s="361"/>
       <c r="C80" s="170" t="s">
         <v>230</v>
       </c>
@@ -5966,7 +5968,7 @@
       <c r="J80" s="238"/>
     </row>
     <row r="81" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A81" s="308"/>
+      <c r="A81" s="353"/>
       <c r="B81" s="242" t="s">
         <v>148</v>
       </c>
@@ -5994,7 +5996,7 @@
       <c r="J81" s="62"/>
     </row>
     <row r="82" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A82" s="308"/>
+      <c r="A82" s="353"/>
       <c r="B82" s="243" t="s">
         <v>168</v>
       </c>
@@ -6022,7 +6024,7 @@
       <c r="J82" s="175"/>
     </row>
     <row r="83" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A83" s="308"/>
+      <c r="A83" s="353"/>
       <c r="B83" s="244" t="s">
         <v>231</v>
       </c>
@@ -6050,7 +6052,7 @@
       <c r="J83" s="62"/>
     </row>
     <row r="84" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A84" s="309"/>
+      <c r="A84" s="354"/>
       <c r="B84" s="241" t="s">
         <v>235</v>
       </c>
@@ -6078,7 +6080,7 @@
       <c r="J84" s="238"/>
     </row>
     <row r="85" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A85" s="304" t="s">
+      <c r="A85" s="289" t="s">
         <v>151</v>
       </c>
       <c r="B85" s="235" t="s">
@@ -6108,8 +6110,8 @@
       <c r="J85" s="231"/>
     </row>
     <row r="86" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A86" s="305"/>
-      <c r="B86" s="301" t="s">
+      <c r="A86" s="291"/>
+      <c r="B86" s="349" t="s">
         <v>193</v>
       </c>
       <c r="C86" s="42" t="s">
@@ -6136,8 +6138,8 @@
       <c r="J86" s="42"/>
     </row>
     <row r="87" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A87" s="305"/>
-      <c r="B87" s="302"/>
+      <c r="A87" s="291"/>
+      <c r="B87" s="350"/>
       <c r="C87" s="42" t="s">
         <v>65</v>
       </c>
@@ -6162,8 +6164,8 @@
       <c r="J87" s="42"/>
     </row>
     <row r="88" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A88" s="305"/>
-      <c r="B88" s="302"/>
+      <c r="A88" s="291"/>
+      <c r="B88" s="350"/>
       <c r="C88" s="42" t="s">
         <v>69</v>
       </c>
@@ -6190,8 +6192,8 @@
       </c>
     </row>
     <row r="89" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A89" s="305"/>
-      <c r="B89" s="303"/>
+      <c r="A89" s="291"/>
+      <c r="B89" s="351"/>
       <c r="C89" s="42" t="s">
         <v>70</v>
       </c>
@@ -6218,7 +6220,7 @@
       </c>
     </row>
     <row r="90" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A90" s="306"/>
+      <c r="A90" s="290"/>
       <c r="B90" s="221" t="s">
         <v>194</v>
       </c>
@@ -6246,13 +6248,13 @@
       <c r="J90" s="22"/>
     </row>
     <row r="91" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A91" s="359" t="s">
+      <c r="A91" s="304" t="s">
         <v>157</v>
       </c>
-      <c r="B91" s="325" t="s">
+      <c r="B91" s="370" t="s">
         <v>152</v>
       </c>
-      <c r="C91" s="323" t="s">
+      <c r="C91" s="368" t="s">
         <v>72</v>
       </c>
       <c r="D91" s="78" t="s">
@@ -6278,9 +6280,9 @@
       </c>
     </row>
     <row r="92" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A92" s="360"/>
-      <c r="B92" s="326"/>
-      <c r="C92" s="324"/>
+      <c r="A92" s="305"/>
+      <c r="B92" s="371"/>
+      <c r="C92" s="369"/>
       <c r="D92" s="80" t="s">
         <v>18</v>
       </c>
@@ -6302,7 +6304,7 @@
       <c r="J92" s="82"/>
     </row>
     <row r="93" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A93" s="360"/>
+      <c r="A93" s="305"/>
       <c r="B93" s="219" t="s">
         <v>153</v>
       </c>
@@ -6330,7 +6332,7 @@
       <c r="J93" s="83"/>
     </row>
     <row r="94" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A94" s="360"/>
+      <c r="A94" s="305"/>
       <c r="B94" s="220" t="s">
         <v>154</v>
       </c>
@@ -6358,7 +6360,7 @@
       <c r="J94" s="83"/>
     </row>
     <row r="95" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A95" s="360"/>
+      <c r="A95" s="305"/>
       <c r="B95" s="220" t="s">
         <v>155</v>
       </c>
@@ -6386,7 +6388,7 @@
       <c r="J95" s="83"/>
     </row>
     <row r="96" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A96" s="361"/>
+      <c r="A96" s="306"/>
       <c r="B96" s="220" t="s">
         <v>156</v>
       </c>
@@ -6416,7 +6418,7 @@
       </c>
     </row>
     <row r="97" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A97" s="304" t="s">
+      <c r="A97" s="289" t="s">
         <v>158</v>
       </c>
       <c r="B97" s="217" t="s">
@@ -6446,7 +6448,7 @@
       <c r="J97" s="42"/>
     </row>
     <row r="98" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A98" s="306"/>
+      <c r="A98" s="290"/>
       <c r="B98" s="218" t="s">
         <v>160</v>
       </c>
@@ -6476,10 +6478,10 @@
       </c>
     </row>
     <row r="99" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A99" s="364" t="s">
+      <c r="A99" s="309" t="s">
         <v>163</v>
       </c>
-      <c r="B99" s="362" t="s">
+      <c r="B99" s="307" t="s">
         <v>161</v>
       </c>
       <c r="C99" s="49" t="s">
@@ -6506,8 +6508,8 @@
       <c r="J99" s="48"/>
     </row>
     <row r="100" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A100" s="365"/>
-      <c r="B100" s="363"/>
+      <c r="A100" s="310"/>
+      <c r="B100" s="308"/>
       <c r="C100" s="51" t="s">
         <v>87</v>
       </c>
@@ -6534,7 +6536,7 @@
       </c>
     </row>
     <row r="101" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A101" s="366"/>
+      <c r="A101" s="311"/>
       <c r="B101" s="114" t="s">
         <v>162</v>
       </c>
@@ -6562,11 +6564,11 @@
       <c r="J101" s="53"/>
     </row>
     <row r="102" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A102" s="304" t="s">
+      <c r="A102" s="289" t="s">
         <v>164</v>
       </c>
       <c r="B102" s="177"/>
-      <c r="C102" s="292" t="s">
+      <c r="C102" s="343" t="s">
         <v>89</v>
       </c>
       <c r="D102" s="39" t="s">
@@ -6590,9 +6592,9 @@
       <c r="J102" s="38"/>
     </row>
     <row r="103" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A103" s="305"/>
+      <c r="A103" s="291"/>
       <c r="B103" s="178"/>
-      <c r="C103" s="293"/>
+      <c r="C103" s="344"/>
       <c r="D103" s="41" t="s">
         <v>18</v>
       </c>
@@ -6616,7 +6618,7 @@
       </c>
     </row>
     <row r="104" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A104" s="306"/>
+      <c r="A104" s="290"/>
       <c r="B104" s="115"/>
       <c r="C104" s="20" t="s">
         <v>90</v>
@@ -6644,7 +6646,7 @@
       </c>
     </row>
     <row r="105" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A105" s="355" t="s">
+      <c r="A105" s="295" t="s">
         <v>165</v>
       </c>
       <c r="B105" s="216" t="s">
@@ -6674,7 +6676,7 @@
       <c r="J105" s="199"/>
     </row>
     <row r="106" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A106" s="356"/>
+      <c r="A106" s="296"/>
       <c r="B106" s="216" t="s">
         <v>167</v>
       </c>
@@ -6702,7 +6704,7 @@
       <c r="J106" s="91"/>
     </row>
     <row r="107" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A107" s="357"/>
+      <c r="A107" s="297"/>
       <c r="B107" s="216" t="s">
         <v>166</v>
       </c>
@@ -6730,7 +6732,7 @@
       <c r="J107" s="89"/>
     </row>
     <row r="108" spans="1:10" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A108" s="294" t="s">
+      <c r="A108" s="298" t="s">
         <v>171</v>
       </c>
       <c r="B108" s="215" t="s">
@@ -6760,7 +6762,7 @@
       <c r="J108" s="42"/>
     </row>
     <row r="109" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A109" s="295"/>
+      <c r="A109" s="299"/>
       <c r="B109" s="180" t="s">
         <v>170</v>
       </c>
@@ -6790,7 +6792,7 @@
       </c>
     </row>
     <row r="110" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A110" s="296"/>
+      <c r="A110" s="300"/>
       <c r="B110" s="226" t="s">
         <v>220</v>
       </c>
@@ -6818,7 +6820,7 @@
       <c r="J110" s="200"/>
     </row>
     <row r="111" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A111" s="310" t="s">
+      <c r="A111" s="355" t="s">
         <v>172</v>
       </c>
       <c r="B111" s="222" t="s">
@@ -6848,7 +6850,7 @@
       <c r="J111" s="225"/>
     </row>
     <row r="112" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A112" s="311"/>
+      <c r="A112" s="356"/>
       <c r="B112" s="116" t="s">
         <v>174</v>
       </c>
@@ -6876,7 +6878,7 @@
       <c r="J112" s="94"/>
     </row>
     <row r="113" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A113" s="304" t="s">
+      <c r="A113" s="289" t="s">
         <v>175</v>
       </c>
       <c r="B113" s="117" t="s">
@@ -6906,7 +6908,7 @@
       <c r="J113" s="43"/>
     </row>
     <row r="114" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A114" s="305"/>
+      <c r="A114" s="291"/>
       <c r="B114" s="181" t="s">
         <v>110</v>
       </c>
@@ -6936,7 +6938,7 @@
       </c>
     </row>
     <row r="115" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A115" s="306"/>
+      <c r="A115" s="290"/>
       <c r="B115" s="230" t="s">
         <v>119</v>
       </c>
@@ -6966,7 +6968,7 @@
       </c>
     </row>
     <row r="116" spans="1:10" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A116" s="294" t="s">
+      <c r="A116" s="298" t="s">
         <v>222</v>
       </c>
       <c r="B116" s="179" t="s">
@@ -6996,7 +6998,7 @@
       <c r="J116" s="42"/>
     </row>
     <row r="117" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A117" s="306"/>
+      <c r="A117" s="290"/>
       <c r="B117" s="113" t="s">
         <v>223</v>
       </c>
@@ -7024,7 +7026,7 @@
       <c r="J117" s="17"/>
     </row>
     <row r="118" spans="1:10" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A118" s="304" t="s">
+      <c r="A118" s="289" t="s">
         <v>250</v>
       </c>
       <c r="B118" s="174" t="s">
@@ -7054,7 +7056,7 @@
       <c r="J118" s="247"/>
     </row>
     <row r="119" spans="1:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A119" s="306"/>
+      <c r="A119" s="290"/>
       <c r="B119" s="113" t="s">
         <v>251</v>
       </c>
@@ -7112,7 +7114,7 @@
       <c r="J120" s="3"/>
     </row>
     <row r="121" spans="1:10" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A121" s="304" t="s">
+      <c r="A121" s="289" t="s">
         <v>179</v>
       </c>
       <c r="B121" s="174" t="s">
@@ -7142,7 +7144,7 @@
       <c r="J121" s="247"/>
     </row>
     <row r="122" spans="1:10" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A122" s="306"/>
+      <c r="A122" s="290"/>
       <c r="B122" s="113" t="s">
         <v>185</v>
       </c>
@@ -7388,11 +7390,11 @@
       <c r="J129" s="43"/>
     </row>
     <row r="130" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A130" s="289" t="s">
+      <c r="A130" s="340" t="s">
         <v>190</v>
       </c>
       <c r="B130" s="182"/>
-      <c r="C130" s="320" t="s">
+      <c r="C130" s="365" t="s">
         <v>132</v>
       </c>
       <c r="D130" s="95" t="s">
@@ -7418,9 +7420,9 @@
       </c>
     </row>
     <row r="131" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A131" s="290"/>
+      <c r="A131" s="341"/>
       <c r="B131" s="182"/>
-      <c r="C131" s="321"/>
+      <c r="C131" s="366"/>
       <c r="D131" s="97" t="s">
         <v>18</v>
       </c>
@@ -7444,9 +7446,9 @@
       </c>
     </row>
     <row r="132" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A132" s="290"/>
+      <c r="A132" s="341"/>
       <c r="B132" s="182"/>
-      <c r="C132" s="321"/>
+      <c r="C132" s="366"/>
       <c r="D132" s="100" t="s">
         <v>18</v>
       </c>
@@ -7470,9 +7472,9 @@
       </c>
     </row>
     <row r="133" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A133" s="290"/>
+      <c r="A133" s="341"/>
       <c r="B133" s="183"/>
-      <c r="C133" s="321"/>
+      <c r="C133" s="366"/>
       <c r="D133" s="100" t="s">
         <v>18</v>
       </c>
@@ -7496,9 +7498,9 @@
       </c>
     </row>
     <row r="134" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A134" s="290"/>
+      <c r="A134" s="341"/>
       <c r="B134" s="184"/>
-      <c r="C134" s="322"/>
+      <c r="C134" s="367"/>
       <c r="D134" s="101" t="s">
         <v>18</v>
       </c>
@@ -7522,9 +7524,9 @@
       </c>
     </row>
     <row r="135" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A135" s="290"/>
+      <c r="A135" s="341"/>
       <c r="B135" s="184"/>
-      <c r="C135" s="287" t="s">
+      <c r="C135" s="338" t="s">
         <v>137</v>
       </c>
       <c r="D135" s="103" t="s">
@@ -7550,9 +7552,9 @@
       </c>
     </row>
     <row r="136" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A136" s="290"/>
+      <c r="A136" s="341"/>
       <c r="B136" s="184"/>
-      <c r="C136" s="288"/>
+      <c r="C136" s="339"/>
       <c r="D136" s="105" t="s">
         <v>18</v>
       </c>
@@ -7576,7 +7578,7 @@
       </c>
     </row>
     <row r="137" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A137" s="291"/>
+      <c r="A137" s="342"/>
       <c r="B137" s="185"/>
       <c r="C137" s="214" t="s">
         <v>139</v>
@@ -7604,7 +7606,7 @@
       </c>
     </row>
     <row r="138" spans="1:10" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A138" s="369" t="s">
+      <c r="A138" s="292" t="s">
         <v>198</v>
       </c>
       <c r="B138" s="149"/>
@@ -7632,7 +7634,7 @@
       <c r="J138" s="19"/>
     </row>
     <row r="139" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A139" s="370"/>
+      <c r="A139" s="293"/>
       <c r="B139" s="150"/>
       <c r="C139" s="2" t="s">
         <v>200</v>
@@ -7658,7 +7660,7 @@
       <c r="J139" s="2"/>
     </row>
     <row r="140" spans="1:10" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A140" s="371"/>
+      <c r="A140" s="294"/>
       <c r="B140" s="152"/>
       <c r="C140" s="25" t="s">
         <v>261</v>
@@ -7684,7 +7686,7 @@
       <c r="J140" s="25"/>
     </row>
     <row r="141" spans="1:10" ht="18.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A141" s="369" t="s">
+      <c r="A141" s="292" t="s">
         <v>206</v>
       </c>
       <c r="B141" s="149"/>
@@ -7712,7 +7714,7 @@
       <c r="J141" s="19"/>
     </row>
     <row r="142" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A142" s="370"/>
+      <c r="A142" s="293"/>
       <c r="B142" s="150"/>
       <c r="C142" s="154" t="s">
         <v>204</v>
@@ -7738,7 +7740,7 @@
       <c r="J142" s="2"/>
     </row>
     <row r="143" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A143" s="371"/>
+      <c r="A143" s="294"/>
       <c r="B143" s="151"/>
       <c r="C143" s="148" t="s">
         <v>205</v>
@@ -7848,7 +7850,7 @@
       <c r="J146" s="6"/>
     </row>
     <row r="147" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A147" s="367" t="s">
+      <c r="A147" s="287" t="s">
         <v>240</v>
       </c>
       <c r="B147" s="248" t="s">
@@ -7878,7 +7880,7 @@
       <c r="J147" s="245"/>
     </row>
     <row r="148" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A148" s="368"/>
+      <c r="A148" s="288"/>
       <c r="B148" s="249" t="s">
         <v>266</v>
       </c>
@@ -9147,34 +9149,6 @@
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="A147:A148"/>
-    <mergeCell ref="A118:A119"/>
-    <mergeCell ref="A113:A115"/>
-    <mergeCell ref="A141:A143"/>
-    <mergeCell ref="A138:A140"/>
-    <mergeCell ref="A105:A107"/>
-    <mergeCell ref="A116:A117"/>
-    <mergeCell ref="A121:A122"/>
-    <mergeCell ref="A2:A27"/>
-    <mergeCell ref="B28:B46"/>
-    <mergeCell ref="A91:A96"/>
-    <mergeCell ref="A97:A98"/>
-    <mergeCell ref="B99:B100"/>
-    <mergeCell ref="A99:A101"/>
-    <mergeCell ref="A102:A104"/>
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="C59:C61"/>
-    <mergeCell ref="A59:A62"/>
-    <mergeCell ref="B2:B11"/>
-    <mergeCell ref="C2:C11"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="A53:A58"/>
-    <mergeCell ref="A28:A51"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="C28:C41"/>
-    <mergeCell ref="C12:C23"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="B12:B27"/>
     <mergeCell ref="C135:C136"/>
     <mergeCell ref="A130:A137"/>
     <mergeCell ref="C102:C103"/>
@@ -9191,6 +9165,34 @@
     <mergeCell ref="C130:C134"/>
     <mergeCell ref="C91:C92"/>
     <mergeCell ref="B91:B92"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="C59:C61"/>
+    <mergeCell ref="A59:A62"/>
+    <mergeCell ref="B2:B11"/>
+    <mergeCell ref="C2:C11"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="A53:A58"/>
+    <mergeCell ref="A28:A51"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="C28:C41"/>
+    <mergeCell ref="C12:C23"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="B12:B27"/>
+    <mergeCell ref="A105:A107"/>
+    <mergeCell ref="A116:A117"/>
+    <mergeCell ref="A121:A122"/>
+    <mergeCell ref="A2:A27"/>
+    <mergeCell ref="B28:B46"/>
+    <mergeCell ref="A91:A96"/>
+    <mergeCell ref="A97:A98"/>
+    <mergeCell ref="B99:B100"/>
+    <mergeCell ref="A99:A101"/>
+    <mergeCell ref="A102:A104"/>
+    <mergeCell ref="A147:A148"/>
+    <mergeCell ref="A118:A119"/>
+    <mergeCell ref="A113:A115"/>
+    <mergeCell ref="A141:A143"/>
+    <mergeCell ref="A138:A140"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9408,9 +9410,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6606E4FC-447B-4C4B-8667-76C225606924}">
   <dimension ref="A1:B100"/>
   <sheetViews>
-    <sheetView topLeftCell="A68" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B83" sqref="B83"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -9420,7 +9420,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>557</v>
       </c>
       <c r="B1" t="s">
         <v>267</v>

</xml_diff>

<commit_message>
update log threads and Table of compounds for kept experiences
</commit_message>
<xml_diff>
--- a/data/Table of compounds_stringent_2025-04-18.xlsx
+++ b/data/Table of compounds_stringent_2025-04-18.xlsx
@@ -5,7 +5,7 @@
   <workbookPr filterPrivacy="1"/>
   <xr:revisionPtr revIDLastSave="688" documentId="11_C9C3E2DFE6E5ECF5CE906EFDC2549BB3DEDA2518" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6C4FBAF6-6931-4CF4-A2F1-5FF3942F2A42}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Experimental Design" sheetId="2" r:id="rId1"/>
@@ -3226,79 +3226,124 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="46" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="10" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="10" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="10" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="50" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="51" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="9" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="9" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="11" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="50" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="11" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="11" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="51" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="10" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="10" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="10" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="46" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="50" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3325,6 +3370,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="11" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="11" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3373,106 +3424,55 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="10" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="10" borderId="46" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="10" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="10" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="10" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="50" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="51" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="11" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="9" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="9" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="50" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="51" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="10" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="10" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="10" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="46" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3938,8 +3938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J271"/>
   <sheetViews>
-    <sheetView topLeftCell="C7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D2" sqref="A2:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="17" x14ac:dyDescent="0.4"/>
@@ -3986,13 +3986,13 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="298" t="s">
+      <c r="A2" s="294" t="s">
         <v>141</v>
       </c>
-      <c r="B2" s="315" t="s">
+      <c r="B2" s="330" t="s">
         <v>140</v>
       </c>
-      <c r="C2" s="318"/>
+      <c r="C2" s="333"/>
       <c r="D2" s="4">
         <v>2</v>
       </c>
@@ -4012,9 +4012,9 @@
       <c r="J2" s="7"/>
     </row>
     <row r="3" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="299"/>
-      <c r="B3" s="316"/>
-      <c r="C3" s="319"/>
+      <c r="A3" s="295"/>
+      <c r="B3" s="331"/>
+      <c r="C3" s="334"/>
       <c r="D3" s="4">
         <v>2</v>
       </c>
@@ -4034,9 +4034,9 @@
       <c r="J3" s="8"/>
     </row>
     <row r="4" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="299"/>
-      <c r="B4" s="316"/>
-      <c r="C4" s="319"/>
+      <c r="A4" s="295"/>
+      <c r="B4" s="331"/>
+      <c r="C4" s="334"/>
       <c r="D4" s="5" t="s">
         <v>10</v>
       </c>
@@ -4056,9 +4056,9 @@
       <c r="J4" s="8"/>
     </row>
     <row r="5" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="299"/>
-      <c r="B5" s="316"/>
-      <c r="C5" s="319"/>
+      <c r="A5" s="295"/>
+      <c r="B5" s="331"/>
+      <c r="C5" s="334"/>
       <c r="D5" s="5" t="s">
         <v>10</v>
       </c>
@@ -4078,9 +4078,9 @@
       <c r="J5" s="8"/>
     </row>
     <row r="6" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="299"/>
-      <c r="B6" s="316"/>
-      <c r="C6" s="319"/>
+      <c r="A6" s="295"/>
+      <c r="B6" s="331"/>
+      <c r="C6" s="334"/>
       <c r="D6" s="5" t="s">
         <v>13</v>
       </c>
@@ -4100,9 +4100,9 @@
       <c r="J6" s="8"/>
     </row>
     <row r="7" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="299"/>
-      <c r="B7" s="316"/>
-      <c r="C7" s="319"/>
+      <c r="A7" s="295"/>
+      <c r="B7" s="331"/>
+      <c r="C7" s="334"/>
       <c r="D7" s="5" t="s">
         <v>13</v>
       </c>
@@ -4122,9 +4122,9 @@
       <c r="J7" s="8"/>
     </row>
     <row r="8" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="299"/>
-      <c r="B8" s="316"/>
-      <c r="C8" s="319"/>
+      <c r="A8" s="295"/>
+      <c r="B8" s="331"/>
+      <c r="C8" s="334"/>
       <c r="D8" s="285"/>
       <c r="E8" s="285"/>
       <c r="F8" t="s">
@@ -4144,9 +4144,9 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="299"/>
-      <c r="B9" s="316"/>
-      <c r="C9" s="320"/>
+      <c r="A9" s="295"/>
+      <c r="B9" s="331"/>
+      <c r="C9" s="335"/>
       <c r="D9" t="s">
         <v>13</v>
       </c>
@@ -4167,9 +4167,9 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="299"/>
-      <c r="B10" s="316"/>
-      <c r="C10" s="320"/>
+      <c r="A10" s="295"/>
+      <c r="B10" s="331"/>
+      <c r="C10" s="335"/>
       <c r="D10" s="202" t="s">
         <v>13</v>
       </c>
@@ -4189,9 +4189,9 @@
       <c r="J10" s="203"/>
     </row>
     <row r="11" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="299"/>
-      <c r="B11" s="317"/>
-      <c r="C11" s="321"/>
+      <c r="A11" s="295"/>
+      <c r="B11" s="332"/>
+      <c r="C11" s="336"/>
       <c r="D11" s="201" t="s">
         <v>13</v>
       </c>
@@ -4211,11 +4211,11 @@
       <c r="J11" s="204"/>
     </row>
     <row r="12" spans="1:10" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="299"/>
-      <c r="B12" s="335" t="s">
+      <c r="A12" s="295"/>
+      <c r="B12" s="352" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="318"/>
+      <c r="C12" s="333"/>
       <c r="D12" s="4" t="s">
         <v>18</v>
       </c>
@@ -4235,9 +4235,9 @@
       <c r="J12" s="7"/>
     </row>
     <row r="13" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="299"/>
-      <c r="B13" s="336"/>
-      <c r="C13" s="332"/>
+      <c r="A13" s="295"/>
+      <c r="B13" s="353"/>
+      <c r="C13" s="349"/>
       <c r="D13" s="5" t="s">
         <v>18</v>
       </c>
@@ -4257,9 +4257,9 @@
       <c r="J13" s="8"/>
     </row>
     <row r="14" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="299"/>
-      <c r="B14" s="336"/>
-      <c r="C14" s="332"/>
+      <c r="A14" s="295"/>
+      <c r="B14" s="353"/>
+      <c r="C14" s="349"/>
       <c r="D14" s="5" t="s">
         <v>18</v>
       </c>
@@ -4279,9 +4279,9 @@
       <c r="J14" s="8"/>
     </row>
     <row r="15" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="299"/>
-      <c r="B15" s="336"/>
-      <c r="C15" s="332"/>
+      <c r="A15" s="295"/>
+      <c r="B15" s="353"/>
+      <c r="C15" s="349"/>
       <c r="D15" s="5" t="s">
         <v>18</v>
       </c>
@@ -4301,9 +4301,9 @@
       <c r="J15" s="8"/>
     </row>
     <row r="16" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="299"/>
-      <c r="B16" s="336"/>
-      <c r="C16" s="332"/>
+      <c r="A16" s="295"/>
+      <c r="B16" s="353"/>
+      <c r="C16" s="349"/>
       <c r="D16" s="5" t="s">
         <v>18</v>
       </c>
@@ -4323,9 +4323,9 @@
       <c r="J16" s="8"/>
     </row>
     <row r="17" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="299"/>
-      <c r="B17" s="336"/>
-      <c r="C17" s="332"/>
+      <c r="A17" s="295"/>
+      <c r="B17" s="353"/>
+      <c r="C17" s="349"/>
       <c r="D17" s="5" t="s">
         <v>18</v>
       </c>
@@ -4345,9 +4345,9 @@
       <c r="J17" s="8"/>
     </row>
     <row r="18" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="299"/>
-      <c r="B18" s="336"/>
-      <c r="C18" s="333"/>
+      <c r="A18" s="295"/>
+      <c r="B18" s="353"/>
+      <c r="C18" s="350"/>
       <c r="D18" s="12" t="s">
         <v>18</v>
       </c>
@@ -4367,9 +4367,9 @@
       <c r="J18" s="13"/>
     </row>
     <row r="19" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="299"/>
-      <c r="B19" s="336"/>
-      <c r="C19" s="333"/>
+      <c r="A19" s="295"/>
+      <c r="B19" s="353"/>
+      <c r="C19" s="350"/>
       <c r="D19" t="s">
         <v>18</v>
       </c>
@@ -4388,9 +4388,9 @@
       <c r="J19" s="284"/>
     </row>
     <row r="20" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="299"/>
-      <c r="B20" s="336"/>
-      <c r="C20" s="333"/>
+      <c r="A20" s="295"/>
+      <c r="B20" s="353"/>
+      <c r="C20" s="350"/>
       <c r="D20" s="24" t="s">
         <v>18</v>
       </c>
@@ -4410,9 +4410,9 @@
       <c r="J20" s="142"/>
     </row>
     <row r="21" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="299"/>
-      <c r="B21" s="336"/>
-      <c r="C21" s="333"/>
+      <c r="A21" s="295"/>
+      <c r="B21" s="353"/>
+      <c r="C21" s="350"/>
       <c r="D21" s="141" t="s">
         <v>18</v>
       </c>
@@ -4432,9 +4432,9 @@
       <c r="J21" s="143"/>
     </row>
     <row r="22" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="299"/>
-      <c r="B22" s="336"/>
-      <c r="C22" s="333"/>
+      <c r="A22" s="295"/>
+      <c r="B22" s="353"/>
+      <c r="C22" s="350"/>
       <c r="D22" s="120" t="s">
         <v>19</v>
       </c>
@@ -4456,9 +4456,9 @@
       </c>
     </row>
     <row r="23" spans="1:10" ht="15.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="299"/>
-      <c r="B23" s="336"/>
-      <c r="C23" s="334"/>
+      <c r="A23" s="295"/>
+      <c r="B23" s="353"/>
+      <c r="C23" s="351"/>
       <c r="D23" s="21" t="s">
         <v>18</v>
       </c>
@@ -4478,8 +4478,8 @@
       <c r="J23" s="142"/>
     </row>
     <row r="24" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="299"/>
-      <c r="B24" s="336"/>
+      <c r="A24" s="295"/>
+      <c r="B24" s="353"/>
       <c r="C24" s="273"/>
       <c r="D24" s="274" t="s">
         <v>18</v>
@@ -4502,8 +4502,8 @@
       </c>
     </row>
     <row r="25" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="299"/>
-      <c r="B25" s="336"/>
+      <c r="A25" s="295"/>
+      <c r="B25" s="353"/>
       <c r="C25" s="273"/>
       <c r="D25" s="274" t="s">
         <v>18</v>
@@ -4526,8 +4526,8 @@
       </c>
     </row>
     <row r="26" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="299"/>
-      <c r="B26" s="336"/>
+      <c r="A26" s="295"/>
+      <c r="B26" s="353"/>
       <c r="C26" s="273"/>
       <c r="D26" s="274" t="s">
         <v>10</v>
@@ -4550,8 +4550,8 @@
       </c>
     </row>
     <row r="27" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="300"/>
-      <c r="B27" s="337"/>
+      <c r="A27" s="296"/>
+      <c r="B27" s="354"/>
       <c r="C27" s="273"/>
       <c r="D27" s="274" t="s">
         <v>10</v>
@@ -4574,13 +4574,13 @@
       </c>
     </row>
     <row r="28" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="325" t="s">
+      <c r="A28" s="342" t="s">
         <v>25</v>
       </c>
-      <c r="B28" s="301" t="s">
+      <c r="B28" s="337" t="s">
         <v>143</v>
       </c>
-      <c r="C28" s="329" t="s">
+      <c r="C28" s="346" t="s">
         <v>24</v>
       </c>
       <c r="D28" s="122" t="s">
@@ -4606,9 +4606,9 @@
       </c>
     </row>
     <row r="29" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="326"/>
-      <c r="B29" s="302"/>
-      <c r="C29" s="330"/>
+      <c r="A29" s="343"/>
+      <c r="B29" s="358"/>
+      <c r="C29" s="347"/>
       <c r="D29" s="124" t="s">
         <v>18</v>
       </c>
@@ -4630,9 +4630,9 @@
       <c r="J29" s="126"/>
     </row>
     <row r="30" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="326"/>
-      <c r="B30" s="302"/>
-      <c r="C30" s="330"/>
+      <c r="A30" s="343"/>
+      <c r="B30" s="358"/>
+      <c r="C30" s="347"/>
       <c r="D30" s="127" t="s">
         <v>18</v>
       </c>
@@ -4654,9 +4654,9 @@
       <c r="J30" s="128"/>
     </row>
     <row r="31" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="326"/>
-      <c r="B31" s="302"/>
-      <c r="C31" s="330"/>
+      <c r="A31" s="343"/>
+      <c r="B31" s="358"/>
+      <c r="C31" s="347"/>
       <c r="D31" s="127" t="s">
         <v>18</v>
       </c>
@@ -4678,9 +4678,9 @@
       <c r="J31" s="128"/>
     </row>
     <row r="32" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="326"/>
-      <c r="B32" s="302"/>
-      <c r="C32" s="330"/>
+      <c r="A32" s="343"/>
+      <c r="B32" s="358"/>
+      <c r="C32" s="347"/>
       <c r="D32" s="127" t="s">
         <v>18</v>
       </c>
@@ -4704,9 +4704,9 @@
       </c>
     </row>
     <row r="33" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="326"/>
-      <c r="B33" s="302"/>
-      <c r="C33" s="330"/>
+      <c r="A33" s="343"/>
+      <c r="B33" s="358"/>
+      <c r="C33" s="347"/>
       <c r="D33" s="127" t="s">
         <v>18</v>
       </c>
@@ -4730,9 +4730,9 @@
       </c>
     </row>
     <row r="34" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="326"/>
-      <c r="B34" s="302"/>
-      <c r="C34" s="330"/>
+      <c r="A34" s="343"/>
+      <c r="B34" s="358"/>
+      <c r="C34" s="347"/>
       <c r="D34" s="127" t="s">
         <v>18</v>
       </c>
@@ -4756,9 +4756,9 @@
       </c>
     </row>
     <row r="35" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="326"/>
-      <c r="B35" s="302"/>
-      <c r="C35" s="330"/>
+      <c r="A35" s="343"/>
+      <c r="B35" s="358"/>
+      <c r="C35" s="347"/>
       <c r="D35" s="165" t="s">
         <v>18</v>
       </c>
@@ -4782,9 +4782,9 @@
       </c>
     </row>
     <row r="36" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="326"/>
-      <c r="B36" s="302"/>
-      <c r="C36" s="330"/>
+      <c r="A36" s="343"/>
+      <c r="B36" s="358"/>
+      <c r="C36" s="347"/>
       <c r="D36" s="165" t="s">
         <v>18</v>
       </c>
@@ -4808,9 +4808,9 @@
       </c>
     </row>
     <row r="37" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="326"/>
-      <c r="B37" s="302"/>
-      <c r="C37" s="330"/>
+      <c r="A37" s="343"/>
+      <c r="B37" s="358"/>
+      <c r="C37" s="347"/>
       <c r="D37" s="165" t="s">
         <v>18</v>
       </c>
@@ -4834,9 +4834,9 @@
       </c>
     </row>
     <row r="38" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="326"/>
-      <c r="B38" s="302"/>
-      <c r="C38" s="330"/>
+      <c r="A38" s="343"/>
+      <c r="B38" s="358"/>
+      <c r="C38" s="347"/>
       <c r="D38" s="165" t="s">
         <v>18</v>
       </c>
@@ -4860,9 +4860,9 @@
       </c>
     </row>
     <row r="39" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="326"/>
-      <c r="B39" s="302"/>
-      <c r="C39" s="330"/>
+      <c r="A39" s="343"/>
+      <c r="B39" s="358"/>
+      <c r="C39" s="347"/>
       <c r="D39" s="165" t="s">
         <v>18</v>
       </c>
@@ -4886,9 +4886,9 @@
       </c>
     </row>
     <row r="40" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="326"/>
-      <c r="B40" s="302"/>
-      <c r="C40" s="330"/>
+      <c r="A40" s="343"/>
+      <c r="B40" s="358"/>
+      <c r="C40" s="347"/>
       <c r="D40" s="165" t="s">
         <v>18</v>
       </c>
@@ -4912,9 +4912,9 @@
       </c>
     </row>
     <row r="41" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A41" s="326"/>
-      <c r="B41" s="302"/>
-      <c r="C41" s="331"/>
+      <c r="A41" s="343"/>
+      <c r="B41" s="358"/>
+      <c r="C41" s="348"/>
       <c r="D41" s="165" t="s">
         <v>73</v>
       </c>
@@ -4938,8 +4938,8 @@
       </c>
     </row>
     <row r="42" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="326"/>
-      <c r="B42" s="302"/>
+      <c r="A42" s="343"/>
+      <c r="B42" s="358"/>
       <c r="C42" s="137" t="s">
         <v>33</v>
       </c>
@@ -4966,8 +4966,8 @@
       </c>
     </row>
     <row r="43" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="326"/>
-      <c r="B43" s="302"/>
+      <c r="A43" s="343"/>
+      <c r="B43" s="358"/>
       <c r="C43" s="186" t="s">
         <v>211</v>
       </c>
@@ -4992,8 +4992,8 @@
       <c r="J43" s="192"/>
     </row>
     <row r="44" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="326"/>
-      <c r="B44" s="302"/>
+      <c r="A44" s="343"/>
+      <c r="B44" s="358"/>
       <c r="C44" s="186" t="s">
         <v>212</v>
       </c>
@@ -5018,8 +5018,8 @@
       <c r="J44" s="192"/>
     </row>
     <row r="45" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="326"/>
-      <c r="B45" s="302"/>
+      <c r="A45" s="343"/>
+      <c r="B45" s="358"/>
       <c r="C45" s="164" t="s">
         <v>213</v>
       </c>
@@ -5044,8 +5044,8 @@
       <c r="J45" s="193"/>
     </row>
     <row r="46" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="326"/>
-      <c r="B46" s="303"/>
+      <c r="A46" s="343"/>
+      <c r="B46" s="338"/>
       <c r="C46" s="280" t="s">
         <v>366</v>
       </c>
@@ -5070,11 +5070,11 @@
       <c r="J46" s="281"/>
     </row>
     <row r="47" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A47" s="326"/>
-      <c r="B47" s="301" t="s">
+      <c r="A47" s="343"/>
+      <c r="B47" s="337" t="s">
         <v>144</v>
       </c>
-      <c r="C47" s="328" t="s">
+      <c r="C47" s="345" t="s">
         <v>30</v>
       </c>
       <c r="D47" s="124" t="s">
@@ -5098,9 +5098,9 @@
       <c r="J47" s="126"/>
     </row>
     <row r="48" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="326"/>
-      <c r="B48" s="303"/>
-      <c r="C48" s="328"/>
+      <c r="A48" s="343"/>
+      <c r="B48" s="338"/>
+      <c r="C48" s="345"/>
       <c r="D48" s="131" t="s">
         <v>18</v>
       </c>
@@ -5122,7 +5122,7 @@
       <c r="J48" s="134"/>
     </row>
     <row r="49" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="326"/>
+      <c r="A49" s="343"/>
       <c r="B49" s="277"/>
       <c r="C49" s="278"/>
       <c r="D49" s="279" t="s">
@@ -5146,7 +5146,7 @@
       <c r="J49" s="281"/>
     </row>
     <row r="50" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="326"/>
+      <c r="A50" s="343"/>
       <c r="B50" s="277"/>
       <c r="C50" s="167" t="s">
         <v>142</v>
@@ -5172,7 +5172,7 @@
       <c r="J50" s="194"/>
     </row>
     <row r="51" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A51" s="327"/>
+      <c r="A51" s="344"/>
       <c r="B51" s="168" t="s">
         <v>145</v>
       </c>
@@ -5230,11 +5230,11 @@
       </c>
     </row>
     <row r="53" spans="1:10" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="322" t="s">
+      <c r="A53" s="339" t="s">
         <v>36</v>
       </c>
       <c r="B53" s="172"/>
-      <c r="C53" s="312" t="s">
+      <c r="C53" s="327" t="s">
         <v>35</v>
       </c>
       <c r="D53" s="63" t="s">
@@ -5258,9 +5258,9 @@
       <c r="J53" s="195"/>
     </row>
     <row r="54" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A54" s="323"/>
+      <c r="A54" s="340"/>
       <c r="B54" s="172"/>
-      <c r="C54" s="313"/>
+      <c r="C54" s="328"/>
       <c r="D54" s="66" t="s">
         <v>18</v>
       </c>
@@ -5282,9 +5282,9 @@
       <c r="J54" s="196"/>
     </row>
     <row r="55" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="323"/>
+      <c r="A55" s="340"/>
       <c r="B55" s="172"/>
-      <c r="C55" s="312" t="s">
+      <c r="C55" s="327" t="s">
         <v>37</v>
       </c>
       <c r="D55" s="63" t="s">
@@ -5308,9 +5308,9 @@
       <c r="J55" s="195"/>
     </row>
     <row r="56" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A56" s="323"/>
+      <c r="A56" s="340"/>
       <c r="B56" s="172"/>
-      <c r="C56" s="313"/>
+      <c r="C56" s="328"/>
       <c r="D56" s="66" t="s">
         <v>18</v>
       </c>
@@ -5332,7 +5332,7 @@
       <c r="J56" s="196"/>
     </row>
     <row r="57" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A57" s="323"/>
+      <c r="A57" s="340"/>
       <c r="B57" s="208"/>
       <c r="C57" s="209" t="s">
         <v>39</v>
@@ -5358,7 +5358,7 @@
       <c r="J57" s="213"/>
     </row>
     <row r="58" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A58" s="324"/>
+      <c r="A58" s="341"/>
       <c r="B58" s="109"/>
       <c r="C58" s="70" t="s">
         <v>215</v>
@@ -5384,11 +5384,11 @@
       <c r="J58" s="72"/>
     </row>
     <row r="59" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="291" t="s">
+      <c r="A59" s="305" t="s">
         <v>44</v>
       </c>
       <c r="B59" s="110"/>
-      <c r="C59" s="314" t="s">
+      <c r="C59" s="329" t="s">
         <v>42</v>
       </c>
       <c r="D59" s="4" t="s">
@@ -5412,9 +5412,9 @@
       <c r="J59" s="198"/>
     </row>
     <row r="60" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A60" s="291"/>
+      <c r="A60" s="305"/>
       <c r="B60" s="110"/>
-      <c r="C60" s="314"/>
+      <c r="C60" s="329"/>
       <c r="D60" s="5" t="s">
         <v>18</v>
       </c>
@@ -5436,9 +5436,9 @@
       <c r="J60" s="8"/>
     </row>
     <row r="61" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A61" s="291"/>
+      <c r="A61" s="305"/>
       <c r="B61" s="110"/>
-      <c r="C61" s="314"/>
+      <c r="C61" s="329"/>
       <c r="D61" s="12" t="s">
         <v>18</v>
       </c>
@@ -5460,7 +5460,7 @@
       <c r="J61" s="12"/>
     </row>
     <row r="62" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A62" s="290"/>
+      <c r="A62" s="306"/>
       <c r="B62" s="173"/>
       <c r="C62" s="36" t="s">
         <v>46</v>
@@ -5486,7 +5486,7 @@
       <c r="J62" s="42"/>
     </row>
     <row r="63" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="345" t="s">
+      <c r="A63" s="297" t="s">
         <v>51</v>
       </c>
       <c r="B63" s="111" t="s">
@@ -5518,7 +5518,7 @@
       </c>
     </row>
     <row r="64" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A64" s="346"/>
+      <c r="A64" s="298"/>
       <c r="B64" s="112" t="s">
         <v>51</v>
       </c>
@@ -5578,13 +5578,13 @@
       </c>
     </row>
     <row r="66" spans="1:10" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A66" s="352" t="s">
+      <c r="A66" s="307" t="s">
         <v>149</v>
       </c>
-      <c r="B66" s="357" t="s">
+      <c r="B66" s="312" t="s">
         <v>146</v>
       </c>
-      <c r="C66" s="362" t="s">
+      <c r="C66" s="317" t="s">
         <v>55</v>
       </c>
       <c r="D66" s="57" t="s">
@@ -5608,9 +5608,9 @@
       <c r="J66" s="57"/>
     </row>
     <row r="67" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="353"/>
-      <c r="B67" s="358"/>
-      <c r="C67" s="363"/>
+      <c r="A67" s="308"/>
+      <c r="B67" s="313"/>
+      <c r="C67" s="318"/>
       <c r="D67" s="46" t="s">
         <v>18</v>
       </c>
@@ -5632,9 +5632,9 @@
       <c r="J67" s="46"/>
     </row>
     <row r="68" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A68" s="353"/>
-      <c r="B68" s="358"/>
-      <c r="C68" s="363"/>
+      <c r="A68" s="308"/>
+      <c r="B68" s="313"/>
+      <c r="C68" s="318"/>
       <c r="D68" s="59" t="s">
         <v>18</v>
       </c>
@@ -5656,9 +5656,9 @@
       <c r="J68" s="59"/>
     </row>
     <row r="69" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A69" s="353"/>
-      <c r="B69" s="359"/>
-      <c r="C69" s="363"/>
+      <c r="A69" s="308"/>
+      <c r="B69" s="314"/>
+      <c r="C69" s="318"/>
       <c r="D69" s="15" t="s">
         <v>18</v>
       </c>
@@ -5682,9 +5682,9 @@
       </c>
     </row>
     <row r="70" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A70" s="353"/>
-      <c r="B70" s="359"/>
-      <c r="C70" s="363"/>
+      <c r="A70" s="308"/>
+      <c r="B70" s="314"/>
+      <c r="C70" s="318"/>
       <c r="D70" s="15" t="s">
         <v>18</v>
       </c>
@@ -5708,9 +5708,9 @@
       </c>
     </row>
     <row r="71" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A71" s="353"/>
-      <c r="B71" s="359"/>
-      <c r="C71" s="363"/>
+      <c r="A71" s="308"/>
+      <c r="B71" s="314"/>
+      <c r="C71" s="318"/>
       <c r="D71" s="15" t="s">
         <v>18</v>
       </c>
@@ -5734,9 +5734,9 @@
       </c>
     </row>
     <row r="72" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A72" s="353"/>
-      <c r="B72" s="359"/>
-      <c r="C72" s="363"/>
+      <c r="A72" s="308"/>
+      <c r="B72" s="314"/>
+      <c r="C72" s="318"/>
       <c r="D72" s="15" t="s">
         <v>18</v>
       </c>
@@ -5760,9 +5760,9 @@
       </c>
     </row>
     <row r="73" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A73" s="353"/>
-      <c r="B73" s="359"/>
-      <c r="C73" s="363"/>
+      <c r="A73" s="308"/>
+      <c r="B73" s="314"/>
+      <c r="C73" s="318"/>
       <c r="D73" s="15" t="s">
         <v>18</v>
       </c>
@@ -5786,9 +5786,9 @@
       </c>
     </row>
     <row r="74" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A74" s="353"/>
-      <c r="B74" s="359"/>
-      <c r="C74" s="364"/>
+      <c r="A74" s="308"/>
+      <c r="B74" s="314"/>
+      <c r="C74" s="319"/>
       <c r="D74" s="15" t="s">
         <v>18</v>
       </c>
@@ -5812,8 +5812,8 @@
       </c>
     </row>
     <row r="75" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A75" s="353"/>
-      <c r="B75" s="359"/>
+      <c r="A75" s="308"/>
+      <c r="B75" s="314"/>
       <c r="C75" s="236" t="s">
         <v>225</v>
       </c>
@@ -5838,8 +5838,8 @@
       <c r="J75" s="233"/>
     </row>
     <row r="76" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A76" s="353"/>
-      <c r="B76" s="360"/>
+      <c r="A76" s="308"/>
+      <c r="B76" s="315"/>
       <c r="C76" s="236" t="s">
         <v>226</v>
       </c>
@@ -5864,11 +5864,11 @@
       <c r="J76" s="233"/>
     </row>
     <row r="77" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A77" s="353"/>
-      <c r="B77" s="357" t="s">
+      <c r="A77" s="308"/>
+      <c r="B77" s="312" t="s">
         <v>147</v>
       </c>
-      <c r="C77" s="347" t="s">
+      <c r="C77" s="299" t="s">
         <v>59</v>
       </c>
       <c r="D77" s="57" t="s">
@@ -5892,9 +5892,9 @@
       <c r="J77" s="57"/>
     </row>
     <row r="78" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A78" s="353"/>
-      <c r="B78" s="358"/>
-      <c r="C78" s="348"/>
+      <c r="A78" s="308"/>
+      <c r="B78" s="313"/>
+      <c r="C78" s="300"/>
       <c r="D78" s="59" t="s">
         <v>18</v>
       </c>
@@ -5916,8 +5916,8 @@
       <c r="J78" s="59"/>
     </row>
     <row r="79" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A79" s="353"/>
-      <c r="B79" s="358"/>
+      <c r="A79" s="308"/>
+      <c r="B79" s="313"/>
       <c r="C79" s="170" t="s">
         <v>229</v>
       </c>
@@ -5942,8 +5942,8 @@
       <c r="J79" s="62"/>
     </row>
     <row r="80" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A80" s="353"/>
-      <c r="B80" s="361"/>
+      <c r="A80" s="308"/>
+      <c r="B80" s="316"/>
       <c r="C80" s="170" t="s">
         <v>230</v>
       </c>
@@ -5968,7 +5968,7 @@
       <c r="J80" s="238"/>
     </row>
     <row r="81" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A81" s="353"/>
+      <c r="A81" s="308"/>
       <c r="B81" s="242" t="s">
         <v>148</v>
       </c>
@@ -5996,7 +5996,7 @@
       <c r="J81" s="62"/>
     </row>
     <row r="82" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A82" s="353"/>
+      <c r="A82" s="308"/>
       <c r="B82" s="243" t="s">
         <v>168</v>
       </c>
@@ -6024,7 +6024,7 @@
       <c r="J82" s="175"/>
     </row>
     <row r="83" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A83" s="353"/>
+      <c r="A83" s="308"/>
       <c r="B83" s="244" t="s">
         <v>231</v>
       </c>
@@ -6052,7 +6052,7 @@
       <c r="J83" s="62"/>
     </row>
     <row r="84" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A84" s="354"/>
+      <c r="A84" s="309"/>
       <c r="B84" s="241" t="s">
         <v>235</v>
       </c>
@@ -6080,7 +6080,7 @@
       <c r="J84" s="238"/>
     </row>
     <row r="85" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A85" s="289" t="s">
+      <c r="A85" s="304" t="s">
         <v>151</v>
       </c>
       <c r="B85" s="235" t="s">
@@ -6110,8 +6110,8 @@
       <c r="J85" s="231"/>
     </row>
     <row r="86" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A86" s="291"/>
-      <c r="B86" s="349" t="s">
+      <c r="A86" s="305"/>
+      <c r="B86" s="301" t="s">
         <v>193</v>
       </c>
       <c r="C86" s="42" t="s">
@@ -6138,8 +6138,8 @@
       <c r="J86" s="42"/>
     </row>
     <row r="87" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A87" s="291"/>
-      <c r="B87" s="350"/>
+      <c r="A87" s="305"/>
+      <c r="B87" s="302"/>
       <c r="C87" s="42" t="s">
         <v>65</v>
       </c>
@@ -6164,8 +6164,8 @@
       <c r="J87" s="42"/>
     </row>
     <row r="88" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A88" s="291"/>
-      <c r="B88" s="350"/>
+      <c r="A88" s="305"/>
+      <c r="B88" s="302"/>
       <c r="C88" s="42" t="s">
         <v>69</v>
       </c>
@@ -6192,8 +6192,8 @@
       </c>
     </row>
     <row r="89" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A89" s="291"/>
-      <c r="B89" s="351"/>
+      <c r="A89" s="305"/>
+      <c r="B89" s="303"/>
       <c r="C89" s="42" t="s">
         <v>70</v>
       </c>
@@ -6220,7 +6220,7 @@
       </c>
     </row>
     <row r="90" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A90" s="290"/>
+      <c r="A90" s="306"/>
       <c r="B90" s="221" t="s">
         <v>194</v>
       </c>
@@ -6248,13 +6248,13 @@
       <c r="J90" s="22"/>
     </row>
     <row r="91" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A91" s="304" t="s">
+      <c r="A91" s="359" t="s">
         <v>157</v>
       </c>
-      <c r="B91" s="370" t="s">
+      <c r="B91" s="325" t="s">
         <v>152</v>
       </c>
-      <c r="C91" s="368" t="s">
+      <c r="C91" s="323" t="s">
         <v>72</v>
       </c>
       <c r="D91" s="78" t="s">
@@ -6280,9 +6280,9 @@
       </c>
     </row>
     <row r="92" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A92" s="305"/>
-      <c r="B92" s="371"/>
-      <c r="C92" s="369"/>
+      <c r="A92" s="360"/>
+      <c r="B92" s="326"/>
+      <c r="C92" s="324"/>
       <c r="D92" s="80" t="s">
         <v>18</v>
       </c>
@@ -6304,7 +6304,7 @@
       <c r="J92" s="82"/>
     </row>
     <row r="93" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A93" s="305"/>
+      <c r="A93" s="360"/>
       <c r="B93" s="219" t="s">
         <v>153</v>
       </c>
@@ -6332,7 +6332,7 @@
       <c r="J93" s="83"/>
     </row>
     <row r="94" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A94" s="305"/>
+      <c r="A94" s="360"/>
       <c r="B94" s="220" t="s">
         <v>154</v>
       </c>
@@ -6360,7 +6360,7 @@
       <c r="J94" s="83"/>
     </row>
     <row r="95" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A95" s="305"/>
+      <c r="A95" s="360"/>
       <c r="B95" s="220" t="s">
         <v>155</v>
       </c>
@@ -6388,7 +6388,7 @@
       <c r="J95" s="83"/>
     </row>
     <row r="96" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A96" s="306"/>
+      <c r="A96" s="361"/>
       <c r="B96" s="220" t="s">
         <v>156</v>
       </c>
@@ -6418,7 +6418,7 @@
       </c>
     </row>
     <row r="97" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A97" s="289" t="s">
+      <c r="A97" s="304" t="s">
         <v>158</v>
       </c>
       <c r="B97" s="217" t="s">
@@ -6448,7 +6448,7 @@
       <c r="J97" s="42"/>
     </row>
     <row r="98" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A98" s="290"/>
+      <c r="A98" s="306"/>
       <c r="B98" s="218" t="s">
         <v>160</v>
       </c>
@@ -6478,10 +6478,10 @@
       </c>
     </row>
     <row r="99" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A99" s="309" t="s">
+      <c r="A99" s="364" t="s">
         <v>163</v>
       </c>
-      <c r="B99" s="307" t="s">
+      <c r="B99" s="362" t="s">
         <v>161</v>
       </c>
       <c r="C99" s="49" t="s">
@@ -6508,8 +6508,8 @@
       <c r="J99" s="48"/>
     </row>
     <row r="100" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A100" s="310"/>
-      <c r="B100" s="308"/>
+      <c r="A100" s="365"/>
+      <c r="B100" s="363"/>
       <c r="C100" s="51" t="s">
         <v>87</v>
       </c>
@@ -6536,7 +6536,7 @@
       </c>
     </row>
     <row r="101" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A101" s="311"/>
+      <c r="A101" s="366"/>
       <c r="B101" s="114" t="s">
         <v>162</v>
       </c>
@@ -6564,11 +6564,11 @@
       <c r="J101" s="53"/>
     </row>
     <row r="102" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A102" s="289" t="s">
+      <c r="A102" s="304" t="s">
         <v>164</v>
       </c>
       <c r="B102" s="177"/>
-      <c r="C102" s="343" t="s">
+      <c r="C102" s="292" t="s">
         <v>89</v>
       </c>
       <c r="D102" s="39" t="s">
@@ -6592,9 +6592,9 @@
       <c r="J102" s="38"/>
     </row>
     <row r="103" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A103" s="291"/>
+      <c r="A103" s="305"/>
       <c r="B103" s="178"/>
-      <c r="C103" s="344"/>
+      <c r="C103" s="293"/>
       <c r="D103" s="41" t="s">
         <v>18</v>
       </c>
@@ -6618,7 +6618,7 @@
       </c>
     </row>
     <row r="104" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A104" s="290"/>
+      <c r="A104" s="306"/>
       <c r="B104" s="115"/>
       <c r="C104" s="20" t="s">
         <v>90</v>
@@ -6646,7 +6646,7 @@
       </c>
     </row>
     <row r="105" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A105" s="295" t="s">
+      <c r="A105" s="355" t="s">
         <v>165</v>
       </c>
       <c r="B105" s="216" t="s">
@@ -6676,7 +6676,7 @@
       <c r="J105" s="199"/>
     </row>
     <row r="106" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A106" s="296"/>
+      <c r="A106" s="356"/>
       <c r="B106" s="216" t="s">
         <v>167</v>
       </c>
@@ -6704,7 +6704,7 @@
       <c r="J106" s="91"/>
     </row>
     <row r="107" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A107" s="297"/>
+      <c r="A107" s="357"/>
       <c r="B107" s="216" t="s">
         <v>166</v>
       </c>
@@ -6732,7 +6732,7 @@
       <c r="J107" s="89"/>
     </row>
     <row r="108" spans="1:10" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A108" s="298" t="s">
+      <c r="A108" s="294" t="s">
         <v>171</v>
       </c>
       <c r="B108" s="215" t="s">
@@ -6762,7 +6762,7 @@
       <c r="J108" s="42"/>
     </row>
     <row r="109" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A109" s="299"/>
+      <c r="A109" s="295"/>
       <c r="B109" s="180" t="s">
         <v>170</v>
       </c>
@@ -6792,7 +6792,7 @@
       </c>
     </row>
     <row r="110" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A110" s="300"/>
+      <c r="A110" s="296"/>
       <c r="B110" s="226" t="s">
         <v>220</v>
       </c>
@@ -6820,7 +6820,7 @@
       <c r="J110" s="200"/>
     </row>
     <row r="111" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A111" s="355" t="s">
+      <c r="A111" s="310" t="s">
         <v>172</v>
       </c>
       <c r="B111" s="222" t="s">
@@ -6850,7 +6850,7 @@
       <c r="J111" s="225"/>
     </row>
     <row r="112" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A112" s="356"/>
+      <c r="A112" s="311"/>
       <c r="B112" s="116" t="s">
         <v>174</v>
       </c>
@@ -6878,7 +6878,7 @@
       <c r="J112" s="94"/>
     </row>
     <row r="113" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A113" s="289" t="s">
+      <c r="A113" s="304" t="s">
         <v>175</v>
       </c>
       <c r="B113" s="117" t="s">
@@ -6908,7 +6908,7 @@
       <c r="J113" s="43"/>
     </row>
     <row r="114" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A114" s="291"/>
+      <c r="A114" s="305"/>
       <c r="B114" s="181" t="s">
         <v>110</v>
       </c>
@@ -6938,7 +6938,7 @@
       </c>
     </row>
     <row r="115" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A115" s="290"/>
+      <c r="A115" s="306"/>
       <c r="B115" s="230" t="s">
         <v>119</v>
       </c>
@@ -6968,7 +6968,7 @@
       </c>
     </row>
     <row r="116" spans="1:10" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A116" s="298" t="s">
+      <c r="A116" s="294" t="s">
         <v>222</v>
       </c>
       <c r="B116" s="179" t="s">
@@ -6998,7 +6998,7 @@
       <c r="J116" s="42"/>
     </row>
     <row r="117" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A117" s="290"/>
+      <c r="A117" s="306"/>
       <c r="B117" s="113" t="s">
         <v>223</v>
       </c>
@@ -7026,7 +7026,7 @@
       <c r="J117" s="17"/>
     </row>
     <row r="118" spans="1:10" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A118" s="289" t="s">
+      <c r="A118" s="304" t="s">
         <v>250</v>
       </c>
       <c r="B118" s="174" t="s">
@@ -7056,7 +7056,7 @@
       <c r="J118" s="247"/>
     </row>
     <row r="119" spans="1:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A119" s="290"/>
+      <c r="A119" s="306"/>
       <c r="B119" s="113" t="s">
         <v>251</v>
       </c>
@@ -7114,7 +7114,7 @@
       <c r="J120" s="3"/>
     </row>
     <row r="121" spans="1:10" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A121" s="289" t="s">
+      <c r="A121" s="304" t="s">
         <v>179</v>
       </c>
       <c r="B121" s="174" t="s">
@@ -7144,7 +7144,7 @@
       <c r="J121" s="247"/>
     </row>
     <row r="122" spans="1:10" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A122" s="290"/>
+      <c r="A122" s="306"/>
       <c r="B122" s="113" t="s">
         <v>185</v>
       </c>
@@ -7390,11 +7390,11 @@
       <c r="J129" s="43"/>
     </row>
     <row r="130" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A130" s="340" t="s">
+      <c r="A130" s="289" t="s">
         <v>190</v>
       </c>
       <c r="B130" s="182"/>
-      <c r="C130" s="365" t="s">
+      <c r="C130" s="320" t="s">
         <v>132</v>
       </c>
       <c r="D130" s="95" t="s">
@@ -7420,9 +7420,9 @@
       </c>
     </row>
     <row r="131" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A131" s="341"/>
+      <c r="A131" s="290"/>
       <c r="B131" s="182"/>
-      <c r="C131" s="366"/>
+      <c r="C131" s="321"/>
       <c r="D131" s="97" t="s">
         <v>18</v>
       </c>
@@ -7446,9 +7446,9 @@
       </c>
     </row>
     <row r="132" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A132" s="341"/>
+      <c r="A132" s="290"/>
       <c r="B132" s="182"/>
-      <c r="C132" s="366"/>
+      <c r="C132" s="321"/>
       <c r="D132" s="100" t="s">
         <v>18</v>
       </c>
@@ -7472,9 +7472,9 @@
       </c>
     </row>
     <row r="133" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A133" s="341"/>
+      <c r="A133" s="290"/>
       <c r="B133" s="183"/>
-      <c r="C133" s="366"/>
+      <c r="C133" s="321"/>
       <c r="D133" s="100" t="s">
         <v>18</v>
       </c>
@@ -7498,9 +7498,9 @@
       </c>
     </row>
     <row r="134" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A134" s="341"/>
+      <c r="A134" s="290"/>
       <c r="B134" s="184"/>
-      <c r="C134" s="367"/>
+      <c r="C134" s="322"/>
       <c r="D134" s="101" t="s">
         <v>18</v>
       </c>
@@ -7524,9 +7524,9 @@
       </c>
     </row>
     <row r="135" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A135" s="341"/>
+      <c r="A135" s="290"/>
       <c r="B135" s="184"/>
-      <c r="C135" s="338" t="s">
+      <c r="C135" s="287" t="s">
         <v>137</v>
       </c>
       <c r="D135" s="103" t="s">
@@ -7552,9 +7552,9 @@
       </c>
     </row>
     <row r="136" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A136" s="341"/>
+      <c r="A136" s="290"/>
       <c r="B136" s="184"/>
-      <c r="C136" s="339"/>
+      <c r="C136" s="288"/>
       <c r="D136" s="105" t="s">
         <v>18</v>
       </c>
@@ -7578,7 +7578,7 @@
       </c>
     </row>
     <row r="137" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A137" s="342"/>
+      <c r="A137" s="291"/>
       <c r="B137" s="185"/>
       <c r="C137" s="214" t="s">
         <v>139</v>
@@ -7606,7 +7606,7 @@
       </c>
     </row>
     <row r="138" spans="1:10" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A138" s="292" t="s">
+      <c r="A138" s="369" t="s">
         <v>198</v>
       </c>
       <c r="B138" s="149"/>
@@ -7634,7 +7634,7 @@
       <c r="J138" s="19"/>
     </row>
     <row r="139" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A139" s="293"/>
+      <c r="A139" s="370"/>
       <c r="B139" s="150"/>
       <c r="C139" s="2" t="s">
         <v>200</v>
@@ -7660,7 +7660,7 @@
       <c r="J139" s="2"/>
     </row>
     <row r="140" spans="1:10" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A140" s="294"/>
+      <c r="A140" s="371"/>
       <c r="B140" s="152"/>
       <c r="C140" s="25" t="s">
         <v>261</v>
@@ -7686,7 +7686,7 @@
       <c r="J140" s="25"/>
     </row>
     <row r="141" spans="1:10" ht="18.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A141" s="292" t="s">
+      <c r="A141" s="369" t="s">
         <v>206</v>
       </c>
       <c r="B141" s="149"/>
@@ -7714,7 +7714,7 @@
       <c r="J141" s="19"/>
     </row>
     <row r="142" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A142" s="293"/>
+      <c r="A142" s="370"/>
       <c r="B142" s="150"/>
       <c r="C142" s="154" t="s">
         <v>204</v>
@@ -7740,7 +7740,7 @@
       <c r="J142" s="2"/>
     </row>
     <row r="143" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A143" s="294"/>
+      <c r="A143" s="371"/>
       <c r="B143" s="151"/>
       <c r="C143" s="148" t="s">
         <v>205</v>
@@ -7850,7 +7850,7 @@
       <c r="J146" s="6"/>
     </row>
     <row r="147" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A147" s="287" t="s">
+      <c r="A147" s="367" t="s">
         <v>240</v>
       </c>
       <c r="B147" s="248" t="s">
@@ -7880,7 +7880,7 @@
       <c r="J147" s="245"/>
     </row>
     <row r="148" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A148" s="288"/>
+      <c r="A148" s="368"/>
       <c r="B148" s="249" t="s">
         <v>266</v>
       </c>
@@ -9149,6 +9149,34 @@
     </row>
   </sheetData>
   <mergeCells count="44">
+    <mergeCell ref="A147:A148"/>
+    <mergeCell ref="A118:A119"/>
+    <mergeCell ref="A113:A115"/>
+    <mergeCell ref="A141:A143"/>
+    <mergeCell ref="A138:A140"/>
+    <mergeCell ref="A105:A107"/>
+    <mergeCell ref="A116:A117"/>
+    <mergeCell ref="A121:A122"/>
+    <mergeCell ref="A2:A27"/>
+    <mergeCell ref="B28:B46"/>
+    <mergeCell ref="A91:A96"/>
+    <mergeCell ref="A97:A98"/>
+    <mergeCell ref="B99:B100"/>
+    <mergeCell ref="A99:A101"/>
+    <mergeCell ref="A102:A104"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="C59:C61"/>
+    <mergeCell ref="A59:A62"/>
+    <mergeCell ref="B2:B11"/>
+    <mergeCell ref="C2:C11"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="A53:A58"/>
+    <mergeCell ref="A28:A51"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="C28:C41"/>
+    <mergeCell ref="C12:C23"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="B12:B27"/>
     <mergeCell ref="C135:C136"/>
     <mergeCell ref="A130:A137"/>
     <mergeCell ref="C102:C103"/>
@@ -9165,34 +9193,6 @@
     <mergeCell ref="C130:C134"/>
     <mergeCell ref="C91:C92"/>
     <mergeCell ref="B91:B92"/>
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="C59:C61"/>
-    <mergeCell ref="A59:A62"/>
-    <mergeCell ref="B2:B11"/>
-    <mergeCell ref="C2:C11"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="A53:A58"/>
-    <mergeCell ref="A28:A51"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="C28:C41"/>
-    <mergeCell ref="C12:C23"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="B12:B27"/>
-    <mergeCell ref="A105:A107"/>
-    <mergeCell ref="A116:A117"/>
-    <mergeCell ref="A121:A122"/>
-    <mergeCell ref="A2:A27"/>
-    <mergeCell ref="B28:B46"/>
-    <mergeCell ref="A91:A96"/>
-    <mergeCell ref="A97:A98"/>
-    <mergeCell ref="B99:B100"/>
-    <mergeCell ref="A99:A101"/>
-    <mergeCell ref="A102:A104"/>
-    <mergeCell ref="A147:A148"/>
-    <mergeCell ref="A118:A119"/>
-    <mergeCell ref="A113:A115"/>
-    <mergeCell ref="A141:A143"/>
-    <mergeCell ref="A138:A140"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9410,7 +9410,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6606E4FC-447B-4C4B-8667-76C225606924}">
   <dimension ref="A1:B100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>